<commit_message>
add: update results table
</commit_message>
<xml_diff>
--- a/Results/Results Table Summary.xlsx
+++ b/Results/Results Table Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University of the Philippines\4th Year 2nd Sem (4.2) LAST SEM!\CS 199\CGE_Ipopt\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81175EDF-9A15-4F5A-852B-B0EC1421438A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86940D8-7747-490B-BFDD-0D6FC52DDB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="4" xr2:uid="{EFB472C8-110D-4341-A8FA-C36916B2E809}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="5" xr2:uid="{EFB472C8-110D-4341-A8FA-C36916B2E809}"/>
   </bookViews>
   <sheets>
     <sheet name="RP5" sheetId="1" r:id="rId1"/>
@@ -133,23 +133,24 @@
     <t>50 YRP</t>
   </si>
   <si>
-    <t>5YRP</t>
+    <t>5YRP (%)</t>
   </si>
   <si>
-    <t>10YRP</t>
+    <t>10YRP (%)</t>
   </si>
   <si>
-    <t>20YRP</t>
+    <t>20YRP (%)</t>
   </si>
   <si>
-    <t>50YRP</t>
+    <t>50YRP (%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -312,7 +313,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -377,26 +378,26 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="1" xr:uid="{4881F658-E921-4900-8925-BE25986AA4F1}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -440,7 +441,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5YRP</c:v>
+                  <c:v>5YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -517,10 +518,10 @@
             <c:numRef>
               <c:f>GraphAllZ!$I$2:$I$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>-1.2486383913803889</c:v>
+                  <c:v>-1.24863839138039</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-4.1514705239347727</c:v>
@@ -585,7 +586,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10YRP</c:v>
+                  <c:v>10YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -662,7 +663,7 @@
             <c:numRef>
               <c:f>GraphAllZ!$J$2:$J$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>-2.1383657719104829</c:v>
@@ -730,7 +731,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20YRP</c:v>
+                  <c:v>20YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -807,7 +808,7 @@
             <c:numRef>
               <c:f>GraphAllZ!$K$2:$K$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>-2.7252180006583622</c:v>
@@ -875,7 +876,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>50YRP</c:v>
+                  <c:v>50YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -952,7 +953,7 @@
             <c:numRef>
               <c:f>GraphAllZ!$L$2:$L$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>-3.1801104497237471</c:v>
@@ -1077,6 +1078,8 @@
         <c:axId val="1095687455"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0"/>
+          <c:min val="-7"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1094,7 +1097,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1242,7 +1245,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5YRP</c:v>
+                  <c:v>5YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1317,10 +1320,10 @@
             <c:numRef>
               <c:f>GraphAllZ!$I$2:$I$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>-1.2486383913803889</c:v>
+                  <c:v>-1.24863839138039</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-4.1514705239347727</c:v>
@@ -1385,7 +1388,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10YRP</c:v>
+                  <c:v>10YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1460,7 +1463,7 @@
             <c:numRef>
               <c:f>GraphAllZ!$J$2:$J$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>-2.1383657719104829</c:v>
@@ -1528,7 +1531,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20YRP</c:v>
+                  <c:v>20YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1603,7 +1606,7 @@
             <c:numRef>
               <c:f>GraphAllZ!$K$2:$K$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>-2.7252180006583622</c:v>
@@ -1671,7 +1674,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>50YRP</c:v>
+                  <c:v>50YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1746,7 +1749,7 @@
             <c:numRef>
               <c:f>GraphAllZ!$L$2:$L$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>-3.1801104497237471</c:v>
@@ -1890,7 +1893,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2037,7 +2040,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5YRP</c:v>
+                  <c:v>5YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2114,7 +2117,7 @@
             <c:numRef>
               <c:f>GraphAllpq!$I$2:$I$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.67935126310307847</c:v>
@@ -2182,7 +2185,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10YRP</c:v>
+                  <c:v>10YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2259,7 +2262,7 @@
             <c:numRef>
               <c:f>GraphAllpq!$J$2:$J$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1.2917769932079051</c:v>
@@ -2327,7 +2330,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20YRP</c:v>
+                  <c:v>20YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2404,7 +2407,7 @@
             <c:numRef>
               <c:f>GraphAllpq!$K$2:$K$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1.668612171819106</c:v>
@@ -2472,7 +2475,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>50YRP</c:v>
+                  <c:v>50YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2549,7 +2552,7 @@
             <c:numRef>
               <c:f>GraphAllpq!$L$2:$L$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1.9551549969719859</c:v>
@@ -2691,7 +2694,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2839,7 +2842,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5YRP</c:v>
+                  <c:v>5YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2914,7 +2917,7 @@
             <c:numRef>
               <c:f>GraphAllpq!$I$2:$I$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.67935126310307847</c:v>
@@ -2982,7 +2985,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10YRP</c:v>
+                  <c:v>10YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3057,7 +3060,7 @@
             <c:numRef>
               <c:f>GraphAllpq!$J$2:$J$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1.2917769932079051</c:v>
@@ -3125,7 +3128,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20YRP</c:v>
+                  <c:v>20YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3200,7 +3203,7 @@
             <c:numRef>
               <c:f>GraphAllpq!$K$2:$K$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1.668612171819106</c:v>
@@ -3268,7 +3271,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>50YRP</c:v>
+                  <c:v>50YRP (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3343,7 +3346,7 @@
             <c:numRef>
               <c:f>GraphAllpq!$L$2:$L$17</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1.9551549969719859</c:v>
@@ -3487,7 +3490,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6259,7 +6262,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H17"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6312,8 +6315,8 @@
       <c r="D2" s="11">
         <v>3371922.167440231</v>
       </c>
-      <c r="E2" s="24">
-        <v>-1.2486383913803889</v>
+      <c r="E2" s="26">
+        <v>-1.24863839138039</v>
       </c>
       <c r="F2" s="11">
         <v>1</v>
@@ -6321,7 +6324,7 @@
       <c r="G2" s="11">
         <v>1.006793512631031</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="26">
         <v>0.67935126310307847</v>
       </c>
     </row>
@@ -6338,7 +6341,7 @@
       <c r="D3" s="13">
         <v>226665.5223881923</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="27">
         <v>-4.1514705239347727</v>
       </c>
       <c r="F3" s="13">
@@ -6347,7 +6350,7 @@
       <c r="G3" s="13">
         <v>1.0053148965906611</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="27">
         <v>0.5314896590661311</v>
       </c>
     </row>
@@ -6364,7 +6367,7 @@
       <c r="D4" s="13">
         <v>10582916.886244269</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="27">
         <v>-1.0311940843691769</v>
       </c>
       <c r="F4" s="13">
@@ -6373,7 +6376,7 @@
       <c r="G4" s="13">
         <v>1.0006148314528269</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="27">
         <v>6.1483145282670293E-2</v>
       </c>
     </row>
@@ -6390,7 +6393,7 @@
       <c r="D5" s="13">
         <v>850694.24528555304</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="27">
         <v>-1.030919189091791</v>
       </c>
       <c r="F5" s="13">
@@ -6399,7 +6402,7 @@
       <c r="G5" s="13">
         <v>1.0048862261331</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="27">
         <v>0.48862261331004131</v>
       </c>
     </row>
@@ -6416,7 +6419,7 @@
       <c r="D6" s="13">
         <v>2929607.8739666371</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="27">
         <v>-0.87804362638689082</v>
       </c>
       <c r="F6" s="13">
@@ -6425,7 +6428,7 @@
       <c r="G6" s="13">
         <v>1.0044124889013271</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="27">
         <v>0.44124889013272828</v>
       </c>
     </row>
@@ -6442,7 +6445,7 @@
       <c r="D7" s="13">
         <v>4154337.916997124</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="27">
         <v>-0.92446232786697857</v>
       </c>
       <c r="F7" s="13">
@@ -6451,7 +6454,7 @@
       <c r="G7" s="13">
         <v>1.000908368828781</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="27">
         <v>9.0836882878120306E-2</v>
       </c>
     </row>
@@ -6468,7 +6471,7 @@
       <c r="D8" s="13">
         <v>1685403.804716252</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="27">
         <v>-1.2195626831614159</v>
       </c>
       <c r="F8" s="13">
@@ -6477,7 +6480,7 @@
       <c r="G8" s="13">
         <v>1.0023475505750179</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="27">
         <v>0.234755057501812</v>
       </c>
     </row>
@@ -6494,7 +6497,7 @@
       <c r="D9" s="13">
         <v>1012958.540185417</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="27">
         <v>-1.016550965859581</v>
       </c>
       <c r="F9" s="13">
@@ -6503,7 +6506,7 @@
       <c r="G9" s="13">
         <v>1.0004503224587791</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="27">
         <v>4.5032245877929533E-2</v>
       </c>
     </row>
@@ -6520,7 +6523,7 @@
       <c r="D10" s="13">
         <v>999576.21799253311</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="27">
         <v>-0.85833767561548846</v>
       </c>
       <c r="F10" s="13">
@@ -6529,7 +6532,7 @@
       <c r="G10" s="13">
         <v>1.0002883997378571</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="27">
         <v>2.8839973785710349E-2</v>
       </c>
     </row>
@@ -6546,7 +6549,7 @@
       <c r="D11" s="13">
         <v>2570935.8422241178</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="27">
         <v>-0.74409806082812757</v>
       </c>
       <c r="F11" s="13">
@@ -6555,7 +6558,7 @@
       <c r="G11" s="13">
         <v>0.99876982636797706</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="27">
         <v>-0.12301736320229351</v>
       </c>
     </row>
@@ -6572,7 +6575,7 @@
       <c r="D12" s="13">
         <v>1416760.3461790089</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="27">
         <v>-0.76990018834614049</v>
       </c>
       <c r="F12" s="13">
@@ -6581,7 +6584,7 @@
       <c r="G12" s="13">
         <v>0.99948953640426397</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="27">
         <v>-5.1046359573603262E-2</v>
       </c>
     </row>
@@ -6598,7 +6601,7 @@
       <c r="D13" s="13">
         <v>1991142.716078849</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="27">
         <v>-0.1162249499211508</v>
       </c>
       <c r="F13" s="13">
@@ -6607,7 +6610,7 @@
       <c r="G13" s="13">
         <v>0.99501288039461622</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="27">
         <v>-0.4987119605383783</v>
       </c>
     </row>
@@ -6624,7 +6627,7 @@
       <c r="D14" s="13">
         <v>1199795.645888966</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="27">
         <v>-0.80500881445908479</v>
       </c>
       <c r="F14" s="13">
@@ -6633,7 +6636,7 @@
       <c r="G14" s="13">
         <v>1.0001441228562129</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="27">
         <v>1.441228562129027E-2</v>
       </c>
     </row>
@@ -6650,7 +6653,7 @@
       <c r="D15" s="13">
         <v>837187.76180597779</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="27">
         <v>-1.2880308943805849</v>
       </c>
       <c r="F15" s="13">
@@ -6659,7 +6662,7 @@
       <c r="G15" s="13">
         <v>1.0052137580091449</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="27">
         <v>0.52137580091453639</v>
       </c>
     </row>
@@ -6676,7 +6679,7 @@
       <c r="D16" s="13">
         <v>445919.93565351359</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="27">
         <v>-0.91189979214244876</v>
       </c>
       <c r="F16" s="13">
@@ -6685,7 +6688,7 @@
       <c r="G16" s="13">
         <v>1.0013206648456929</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="27">
         <v>0.13206648456931541</v>
       </c>
     </row>
@@ -6702,7 +6705,7 @@
       <c r="D17" s="14">
         <v>541529.11506716756</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="28">
         <v>-0.77902729645167235</v>
       </c>
       <c r="F17" s="14">
@@ -6711,7 +6714,7 @@
       <c r="G17" s="14">
         <v>0.99998728520090896</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="28">
         <v>-1.2714799091040341E-3</v>
       </c>
     </row>
@@ -6730,7 +6733,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H17"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6783,7 +6786,7 @@
       <c r="D2" s="11">
         <v>3341541.9131478579</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="26">
         <v>-2.1383657719104829</v>
       </c>
       <c r="F2" s="11">
@@ -6792,7 +6795,7 @@
       <c r="G2" s="11">
         <v>1.012917769932079</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="26">
         <v>1.2917769932079051</v>
       </c>
     </row>
@@ -6809,7 +6812,7 @@
       <c r="D3" s="13">
         <v>227221.33319504379</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="27">
         <v>-3.91643853520387</v>
       </c>
       <c r="F3" s="13">
@@ -6818,7 +6821,7 @@
       <c r="G3" s="13">
         <v>1.003798874193214</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="27">
         <v>0.37988741932137859</v>
       </c>
     </row>
@@ -6835,7 +6838,7 @@
       <c r="D4" s="13">
         <v>10509452.422878619</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="27">
         <v>-1.7182154693695459</v>
       </c>
       <c r="F4" s="13">
@@ -6844,7 +6847,7 @@
       <c r="G4" s="13">
         <v>1.001162373313975</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="27">
         <v>0.1162373313974507</v>
       </c>
     </row>
@@ -6861,7 +6864,7 @@
       <c r="D5" s="13">
         <v>845128.35955597402</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="27">
         <v>-1.678449835511155</v>
       </c>
       <c r="F5" s="13">
@@ -6870,7 +6873,7 @@
       <c r="G5" s="13">
         <v>1.008459584605764</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="27">
         <v>0.84595846057635704</v>
       </c>
     </row>
@@ -6887,7 +6890,7 @@
       <c r="D6" s="13">
         <v>2911148.510167181</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="27">
         <v>-1.502607845193729</v>
       </c>
       <c r="F6" s="13">
@@ -6896,7 +6899,7 @@
       <c r="G6" s="13">
         <v>1.0081943577466219</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="27">
         <v>0.81943577466219164</v>
       </c>
     </row>
@@ -6913,7 +6916,7 @@
       <c r="D7" s="13">
         <v>4129223.5030272719</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="27">
         <v>-1.5234083253033479</v>
       </c>
       <c r="F7" s="13">
@@ -6922,7 +6925,7 @@
       <c r="G7" s="13">
         <v>1.0016865944369291</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="27">
         <v>0.16865944369286459</v>
       </c>
     </row>
@@ -6939,7 +6942,7 @@
       <c r="D8" s="13">
         <v>1676461.958796306</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="27">
         <v>-1.7436385443409941</v>
       </c>
       <c r="F8" s="13">
@@ -6948,7 +6951,7 @@
       <c r="G8" s="13">
         <v>1.00249362696532</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="27">
         <v>0.2493626965320184</v>
       </c>
     </row>
@@ -6965,7 +6968,7 @@
       <c r="D9" s="13">
         <v>1001988.3664715179</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="27">
         <v>-2.0885253731306759</v>
       </c>
       <c r="F9" s="13">
@@ -6974,7 +6977,7 @@
       <c r="G9" s="13">
         <v>1.001636849992205</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="27">
         <v>0.16368499922048141</v>
       </c>
     </row>
@@ -6991,7 +6994,7 @@
       <c r="D10" s="13">
         <v>993776.97677164082</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="27">
         <v>-1.4335278457198051</v>
       </c>
       <c r="F10" s="13">
@@ -7000,7 +7003,7 @@
       <c r="G10" s="13">
         <v>1.0008872351841169</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="27">
         <v>8.8723518411693014E-2</v>
       </c>
     </row>
@@ -7017,7 +7020,7 @@
       <c r="D11" s="13">
         <v>2560737.5522944559</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="27">
         <v>-1.137822574906268</v>
       </c>
       <c r="F11" s="13">
@@ -7026,7 +7029,7 @@
       <c r="G11" s="13">
         <v>0.99729562129493587</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="27">
         <v>-0.27043787050641249</v>
       </c>
     </row>
@@ -7043,7 +7046,7 @@
       <c r="D12" s="13">
         <v>1409554.0075849199</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="27">
         <v>-1.2746331870474441</v>
       </c>
       <c r="F12" s="13">
@@ -7052,7 +7055,7 @@
       <c r="G12" s="13">
         <v>0.9999122537008962</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="27">
         <v>-8.7746299103796943E-3</v>
       </c>
     </row>
@@ -7069,7 +7072,7 @@
       <c r="D13" s="13">
         <v>1989601.208189657</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="27">
         <v>-0.1935532227760586</v>
       </c>
       <c r="F13" s="13">
@@ -7078,7 +7081,7 @@
       <c r="G13" s="13">
         <v>0.99212034660887516</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="27">
         <v>-0.78796533911248412</v>
       </c>
     </row>
@@ -7095,7 +7098,7 @@
       <c r="D14" s="13">
         <v>1194876.7203289799</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="27">
         <v>-1.211688718021857</v>
       </c>
       <c r="F14" s="13">
@@ -7104,7 +7107,7 @@
       <c r="G14" s="13">
         <v>0.99958063770216132</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="27">
         <v>-4.1936229783867678E-2</v>
       </c>
     </row>
@@ -7121,7 +7124,7 @@
       <c r="D15" s="13">
         <v>830311.32811358734</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="27">
         <v>-2.0988242924300402</v>
       </c>
       <c r="F15" s="13">
@@ -7130,7 +7133,7 @@
       <c r="G15" s="13">
         <v>1.008953129550731</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="27">
         <v>0.89531295507314645</v>
       </c>
     </row>
@@ -7147,7 +7150,7 @@
       <c r="D16" s="13">
         <v>443710.5555951579</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="27">
         <v>-1.4028472809528549</v>
       </c>
       <c r="F16" s="13">
@@ -7156,7 +7159,7 @@
       <c r="G16" s="13">
         <v>1.001668892972801</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="27">
         <v>0.1668892972801039</v>
       </c>
     </row>
@@ -7173,7 +7176,7 @@
       <c r="D17" s="14">
         <v>540641.74227424012</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="28">
         <v>-0.94161503036142447</v>
       </c>
       <c r="F17" s="14">
@@ -7182,7 +7185,7 @@
       <c r="G17" s="14">
         <v>0.99748560239649309</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="28">
         <v>-0.25143976035069132</v>
       </c>
     </row>
@@ -7254,7 +7257,7 @@
       <c r="D2" s="11">
         <v>3321503.50550575</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="26">
         <v>-2.7252180006583622</v>
       </c>
       <c r="F2" s="11">
@@ -7263,7 +7266,7 @@
       <c r="G2" s="11">
         <v>1.0166861217181911</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="26">
         <v>1.668612171819106</v>
       </c>
     </row>
@@ -7280,7 +7283,7 @@
       <c r="D3" s="13">
         <v>224487.88262577329</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="27">
         <v>-5.0723144474274706</v>
       </c>
       <c r="F3" s="13">
@@ -7289,7 +7292,7 @@
       <c r="G3" s="13">
         <v>1.00503360265802</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="27">
         <v>0.50336026580204418</v>
       </c>
     </row>
@@ -7306,7 +7309,7 @@
       <c r="D4" s="13">
         <v>10459697.821077229</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="27">
         <v>-2.183508127529918</v>
       </c>
       <c r="F4" s="13">
@@ -7315,7 +7318,7 @@
       <c r="G4" s="13">
         <v>1.0014870634100901</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="27">
         <v>0.1487063410090084</v>
       </c>
     </row>
@@ -7332,7 +7335,7 @@
       <c r="D5" s="13">
         <v>841300.77145803953</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="27">
         <v>-2.123748340672893</v>
       </c>
       <c r="F5" s="13">
@@ -7341,7 +7344,7 @@
       <c r="G5" s="13">
         <v>1.010567877235488</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="27">
         <v>1.0567877235487579</v>
       </c>
     </row>
@@ -7358,7 +7361,7 @@
       <c r="D6" s="13">
         <v>2899175.4909311002</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="27">
         <v>-1.907709531643097</v>
       </c>
       <c r="F6" s="13">
@@ -7367,7 +7370,7 @@
       <c r="G6" s="13">
         <v>1.0104476900192421</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="27">
         <v>1.044769001924206</v>
       </c>
     </row>
@@ -7384,7 +7387,7 @@
       <c r="D7" s="13">
         <v>4112278.113780838</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="27">
         <v>-1.92753374413003</v>
       </c>
       <c r="F7" s="13">
@@ -7393,7 +7396,7 @@
       <c r="G7" s="13">
         <v>1.0020525062501811</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="27">
         <v>0.2052506250181052</v>
       </c>
     </row>
@@ -7410,7 +7413,7 @@
       <c r="D8" s="13">
         <v>1668390.1823580919</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="27">
         <v>-2.2167201905669121</v>
       </c>
       <c r="F8" s="13">
@@ -7419,7 +7422,7 @@
       <c r="G8" s="13">
         <v>1.003201308149122</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="27">
         <v>0.32013081491217837</v>
       </c>
     </row>
@@ -7436,7 +7439,7 @@
       <c r="D9" s="13">
         <v>996378.48776528169</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="27">
         <v>-2.6367068839995902</v>
       </c>
       <c r="F9" s="13">
@@ -7445,7 +7448,7 @@
       <c r="G9" s="13">
         <v>1.002059458994091</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="27">
         <v>0.20594589940907679</v>
       </c>
     </row>
@@ -7462,7 +7465,7 @@
       <c r="D10" s="13">
         <v>989860.45310062566</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="27">
         <v>-1.821983133358656</v>
       </c>
       <c r="F10" s="13">
@@ -7471,7 +7474,7 @@
       <c r="G10" s="13">
         <v>1.0011499607302461</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="27">
         <v>0.11499607302458691</v>
       </c>
     </row>
@@ -7488,7 +7491,7 @@
       <c r="D11" s="13">
         <v>2552921.4062267612</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="27">
         <v>-1.4395798630096761</v>
       </c>
       <c r="F11" s="13">
@@ -7497,7 +7500,7 @@
       <c r="G11" s="13">
         <v>0.99649538557265627</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="27">
         <v>-0.3504614427343733</v>
       </c>
     </row>
@@ -7514,7 +7517,7 @@
       <c r="D12" s="13">
         <v>1404718.853545398</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="27">
         <v>-1.6132880761686019</v>
       </c>
       <c r="F12" s="13">
@@ -7523,7 +7526,7 @@
       <c r="G12" s="13">
         <v>0.99984109256913878</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="27">
         <v>-1.589074308612215E-2</v>
       </c>
     </row>
@@ -7540,7 +7543,7 @@
       <c r="D13" s="13">
         <v>1988837.9122553931</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="27">
         <v>-0.23184323522921629</v>
       </c>
       <c r="F13" s="13">
@@ -7549,7 +7552,7 @@
       <c r="G13" s="13">
         <v>0.98992436344360857</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="27">
         <v>-1.007563655639143</v>
       </c>
     </row>
@@ -7566,7 +7569,7 @@
       <c r="D14" s="13">
         <v>1190960.3980956699</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="27">
         <v>-1.535476815389939</v>
       </c>
       <c r="F14" s="13">
@@ -7575,7 +7578,7 @@
       <c r="G14" s="13">
         <v>0.99943587891029384</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="27">
         <v>-5.6412108970615993E-2</v>
       </c>
     </row>
@@ -7592,7 +7595,7 @@
       <c r="D15" s="13">
         <v>825489.36248479248</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="27">
         <v>-2.6673774221976831</v>
       </c>
       <c r="F15" s="13">
@@ -7601,7 +7604,7 @@
       <c r="G15" s="13">
         <v>1.0114747019397261</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="27">
         <v>1.1474701939726111</v>
       </c>
     </row>
@@ -7618,7 +7621,7 @@
       <c r="D16" s="13">
         <v>442004.56013159722</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="27">
         <v>-1.781937417839673</v>
       </c>
       <c r="F16" s="13">
@@ -7627,7 +7630,7 @@
       <c r="G16" s="13">
         <v>1.0021373425458939</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="27">
         <v>0.21373425458937059</v>
       </c>
     </row>
@@ -7644,7 +7647,7 @@
       <c r="D17" s="14">
         <v>539281.02177879063</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="28">
         <v>-1.190931285719933</v>
       </c>
       <c r="F17" s="14">
@@ -7653,7 +7656,7 @@
       <c r="G17" s="14">
         <v>0.99676580550532046</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="28">
         <v>-0.32341944946795431</v>
       </c>
     </row>
@@ -7672,7 +7675,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H17"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7725,7 +7728,7 @@
       <c r="D2" s="11">
         <v>3305970.940609239</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="26">
         <v>-3.1801104497237471</v>
       </c>
       <c r="F2" s="11">
@@ -7734,8 +7737,8 @@
       <c r="G2" s="11">
         <v>1.0195515499697201</v>
       </c>
-      <c r="H2" s="24">
-        <v>1.9551549969719859</v>
+      <c r="H2" s="26">
+        <v>1.9551549969719899</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -7751,7 +7754,7 @@
       <c r="D3" s="13">
         <v>222151.59597603261</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="27">
         <v>-6.0602443163058473</v>
       </c>
       <c r="F3" s="13">
@@ -7760,7 +7763,7 @@
       <c r="G3" s="13">
         <v>1.0061509444978629</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="27">
         <v>0.61509444978633532</v>
       </c>
     </row>
@@ -7777,7 +7780,7 @@
       <c r="D4" s="13">
         <v>10420343.124573519</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="27">
         <v>-2.5515434586215591</v>
       </c>
       <c r="F4" s="13">
@@ -7786,7 +7789,7 @@
       <c r="G4" s="13">
         <v>1.001743645504285</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="27">
         <v>0.17436455042851851</v>
       </c>
     </row>
@@ -7803,7 +7806,7 @@
       <c r="D5" s="13">
         <v>838157.32115848304</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="27">
         <v>-2.489454807415771</v>
       </c>
       <c r="F5" s="13">
@@ -7812,7 +7815,7 @@
       <c r="G5" s="13">
         <v>1.0126732860578029</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="27">
         <v>1.2673286057802711</v>
       </c>
     </row>
@@ -7829,7 +7832,7 @@
       <c r="D6" s="13">
         <v>2888980.153776777</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="27">
         <v>-2.252664149496697</v>
       </c>
       <c r="F6" s="13">
@@ -7838,7 +7841,7 @@
       <c r="G6" s="13">
         <v>1.012511883395971</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="27">
         <v>1.251188339597076</v>
       </c>
     </row>
@@ -7855,7 +7858,7 @@
       <c r="D7" s="13">
         <v>4099208.7994941161</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="27">
         <v>-2.2392198336667861</v>
       </c>
       <c r="F7" s="13">
@@ -7864,7 +7867,7 @@
       <c r="G7" s="13">
         <v>1.0022260059102099</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="27">
         <v>0.22260059102101601</v>
       </c>
     </row>
@@ -7881,7 +7884,7 @@
       <c r="D8" s="13">
         <v>1661980.2115839471</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="27">
         <v>-2.5924044713821921</v>
       </c>
       <c r="F8" s="13">
@@ -7890,7 +7893,7 @@
       <c r="G8" s="13">
         <v>1.003783197101296</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="27">
         <v>0.37831971012955989</v>
       </c>
     </row>
@@ -7907,7 +7910,7 @@
       <c r="D9" s="13">
         <v>992376.37968712253</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="27">
         <v>-3.0277815877195242</v>
       </c>
       <c r="F9" s="13">
@@ -7916,7 +7919,7 @@
       <c r="G9" s="13">
         <v>1.002317138439438</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="27">
         <v>0.23171384394375941</v>
       </c>
     </row>
@@ -7933,7 +7936,7 @@
       <c r="D10" s="13">
         <v>986770.41759965976</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="27">
         <v>-2.1284642707574348</v>
       </c>
       <c r="F10" s="13">
@@ -7942,8 +7945,8 @@
       <c r="G10" s="13">
         <v>1.001348230429324</v>
       </c>
-      <c r="H10" s="25">
-        <v>0.13482304293244149</v>
+      <c r="H10" s="27">
+        <v>0.13482304293244099</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -7959,7 +7962,7 @@
       <c r="D11" s="13">
         <v>2546392.320697932</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="27">
         <v>-1.6916477140849879</v>
       </c>
       <c r="F11" s="13">
@@ -7968,7 +7971,7 @@
       <c r="G11" s="13">
         <v>0.99602838625735035</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="27">
         <v>-0.39716137426496489</v>
       </c>
     </row>
@@ -7985,7 +7988,7 @@
       <c r="D12" s="13">
         <v>1400922.8080737151</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="27">
         <v>-1.8791636507218989</v>
       </c>
       <c r="F12" s="13">
@@ -7994,7 +7997,7 @@
       <c r="G12" s="13">
         <v>0.99974891627420936</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="27">
         <v>-2.5108372579063509E-2</v>
       </c>
     </row>
@@ -8011,7 +8014,7 @@
       <c r="D13" s="13">
         <v>1987894.658411968</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="27">
         <v>-0.27916066453800431</v>
       </c>
       <c r="F13" s="13">
@@ -8020,7 +8023,7 @@
       <c r="G13" s="13">
         <v>0.98827503641633296</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="27">
         <v>-1.1724963583667041</v>
       </c>
     </row>
@@ -8037,7 +8040,7 @@
       <c r="D14" s="13">
         <v>1187636.052603103</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="27">
         <v>-1.810322305088782</v>
       </c>
       <c r="F14" s="13">
@@ -8046,7 +8049,7 @@
       <c r="G14" s="13">
         <v>0.99951767325548246</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="27">
         <v>-4.823267445175361E-2</v>
       </c>
     </row>
@@ -8063,7 +8066,7 @@
       <c r="D15" s="13">
         <v>821592.0268113811</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="27">
         <v>-3.1269083615393072</v>
       </c>
       <c r="F15" s="13">
@@ -8072,7 +8075,7 @@
       <c r="G15" s="13">
         <v>1.013604556016358</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="27">
         <v>1.3604556016357789</v>
       </c>
     </row>
@@ -8089,7 +8092,7 @@
       <c r="D16" s="13">
         <v>440612.6737071859</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="27">
         <v>-2.0912292222033848</v>
       </c>
       <c r="F16" s="13">
@@ -8098,7 +8101,7 @@
       <c r="G16" s="13">
         <v>1.0026263687291741</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="27">
         <v>0.2626368729173878</v>
       </c>
     </row>
@@ -8115,7 +8118,7 @@
       <c r="D17" s="14">
         <v>538165.00742780615</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="28">
         <v>-1.3954115738057631</v>
       </c>
       <c r="F17" s="14">
@@ -8124,7 +8127,7 @@
       <c r="G17" s="14">
         <v>0.99627262771394098</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="28">
         <v>-0.37273722860590158</v>
       </c>
     </row>
@@ -8142,7 +8145,629 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0995742D-E9FB-4948-9F3D-6BB4E302B1C3}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>3414557.6450926722</v>
+      </c>
+      <c r="C2" s="11">
+        <v>3371922.167440231</v>
+      </c>
+      <c r="D2" s="11">
+        <v>3341541.9131478579</v>
+      </c>
+      <c r="E2" s="11">
+        <v>3321503.50550575</v>
+      </c>
+      <c r="F2" s="11">
+        <v>3305970.940609239</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="26">
+        <v>-1.24863839138039</v>
+      </c>
+      <c r="J2" s="26">
+        <v>-2.1383657719104829</v>
+      </c>
+      <c r="K2" s="26">
+        <v>-2.7252180006583622</v>
+      </c>
+      <c r="L2" s="26">
+        <v>-3.1801104497237471</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13">
+        <v>236483.0463515812</v>
+      </c>
+      <c r="C3" s="13">
+        <v>226665.5223881923</v>
+      </c>
+      <c r="D3" s="13">
+        <v>227221.33319504379</v>
+      </c>
+      <c r="E3" s="13">
+        <v>224487.88262577329</v>
+      </c>
+      <c r="F3" s="13">
+        <v>222151.59597603261</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="27">
+        <v>-4.1514705239347727</v>
+      </c>
+      <c r="J3" s="27">
+        <v>-3.91643853520387</v>
+      </c>
+      <c r="K3" s="27">
+        <v>-5.0723144474274706</v>
+      </c>
+      <c r="L3" s="27">
+        <v>-6.0602443163058473</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13">
+        <v>10693184.370907759</v>
+      </c>
+      <c r="C4" s="13">
+        <v>10582916.886244269</v>
+      </c>
+      <c r="D4" s="13">
+        <v>10509452.422878619</v>
+      </c>
+      <c r="E4" s="13">
+        <v>10459697.821077229</v>
+      </c>
+      <c r="F4" s="13">
+        <v>10420343.124573519</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="27">
+        <v>-1.0311940843691769</v>
+      </c>
+      <c r="J4" s="27">
+        <v>-1.7182154693695459</v>
+      </c>
+      <c r="K4" s="27">
+        <v>-2.183508127529918</v>
+      </c>
+      <c r="L4" s="27">
+        <v>-2.5515434586215591</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13">
+        <v>859555.56858298206</v>
+      </c>
+      <c r="C5" s="13">
+        <v>850694.24528555304</v>
+      </c>
+      <c r="D5" s="13">
+        <v>845128.35955597402</v>
+      </c>
+      <c r="E5" s="13">
+        <v>841300.77145803953</v>
+      </c>
+      <c r="F5" s="13">
+        <v>838157.32115848304</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="27">
+        <v>-1.030919189091791</v>
+      </c>
+      <c r="J5" s="27">
+        <v>-1.678449835511155</v>
+      </c>
+      <c r="K5" s="27">
+        <v>-2.123748340672893</v>
+      </c>
+      <c r="L5" s="27">
+        <v>-2.489454807415771</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13">
+        <v>2955558.9711368098</v>
+      </c>
+      <c r="C6" s="13">
+        <v>2929607.8739666371</v>
+      </c>
+      <c r="D6" s="13">
+        <v>2911148.510167181</v>
+      </c>
+      <c r="E6" s="13">
+        <v>2899175.4909311002</v>
+      </c>
+      <c r="F6" s="13">
+        <v>2888980.153776777</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="27">
+        <v>-0.87804362638689082</v>
+      </c>
+      <c r="J6" s="27">
+        <v>-1.502607845193729</v>
+      </c>
+      <c r="K6" s="27">
+        <v>-1.907709531643097</v>
+      </c>
+      <c r="L6" s="27">
+        <v>-2.252664149496697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13">
+        <v>4193101.5613005492</v>
+      </c>
+      <c r="C7" s="13">
+        <v>4154337.916997124</v>
+      </c>
+      <c r="D7" s="13">
+        <v>4129223.5030272719</v>
+      </c>
+      <c r="E7" s="13">
+        <v>4112278.113780838</v>
+      </c>
+      <c r="F7" s="13">
+        <v>4099208.7994941161</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="27">
+        <v>-0.92446232786697857</v>
+      </c>
+      <c r="J7" s="27">
+        <v>-1.5234083253033479</v>
+      </c>
+      <c r="K7" s="27">
+        <v>-1.92753374413003</v>
+      </c>
+      <c r="L7" s="27">
+        <v>-2.2392198336667861</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13">
+        <v>1706212.1311634949</v>
+      </c>
+      <c r="C8" s="13">
+        <v>1685403.804716252</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1676461.958796306</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1668390.1823580919</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1661980.2115839471</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="27">
+        <v>-1.2195626831614159</v>
+      </c>
+      <c r="J8" s="27">
+        <v>-1.7436385443409941</v>
+      </c>
+      <c r="K8" s="27">
+        <v>-2.2167201905669121</v>
+      </c>
+      <c r="L8" s="27">
+        <v>-2.5924044713821921</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13">
+        <v>1023361.531720356</v>
+      </c>
+      <c r="C9" s="13">
+        <v>1012958.540185417</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1001988.3664715179</v>
+      </c>
+      <c r="E9" s="13">
+        <v>996378.48776528169</v>
+      </c>
+      <c r="F9" s="13">
+        <v>992376.37968712253</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="27">
+        <v>-1.016550965859581</v>
+      </c>
+      <c r="J9" s="27">
+        <v>-2.0885253731306759</v>
+      </c>
+      <c r="K9" s="27">
+        <v>-2.6367068839995902</v>
+      </c>
+      <c r="L9" s="27">
+        <v>-3.0277815877195242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1008230.237982081</v>
+      </c>
+      <c r="C10" s="13">
+        <v>999576.21799253311</v>
+      </c>
+      <c r="D10" s="13">
+        <v>993776.97677164082</v>
+      </c>
+      <c r="E10" s="13">
+        <v>989860.45310062566</v>
+      </c>
+      <c r="F10" s="13">
+        <v>986770.41759965976</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="27">
+        <v>-0.85833767561548846</v>
+      </c>
+      <c r="J10" s="27">
+        <v>-1.4335278457198051</v>
+      </c>
+      <c r="K10" s="27">
+        <v>-1.821983133358656</v>
+      </c>
+      <c r="L10" s="27">
+        <v>-2.1284642707574348</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13">
+        <v>2590209.541191509</v>
+      </c>
+      <c r="C11" s="13">
+        <v>2570935.8422241178</v>
+      </c>
+      <c r="D11" s="13">
+        <v>2560737.5522944559</v>
+      </c>
+      <c r="E11" s="13">
+        <v>2552921.4062267612</v>
+      </c>
+      <c r="F11" s="13">
+        <v>2546392.320697932</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="27">
+        <v>-0.74409806082812757</v>
+      </c>
+      <c r="J11" s="27">
+        <v>-1.137822574906268</v>
+      </c>
+      <c r="K11" s="27">
+        <v>-1.4395798630096761</v>
+      </c>
+      <c r="L11" s="27">
+        <v>-1.6916477140849879</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13">
+        <v>1427752.6162607169</v>
+      </c>
+      <c r="C12" s="13">
+        <v>1416760.3461790089</v>
+      </c>
+      <c r="D12" s="13">
+        <v>1409554.0075849199</v>
+      </c>
+      <c r="E12" s="13">
+        <v>1404718.853545398</v>
+      </c>
+      <c r="F12" s="13">
+        <v>1400922.8080737151</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="27">
+        <v>-0.76990018834614049</v>
+      </c>
+      <c r="J12" s="27">
+        <v>-1.2746331870474441</v>
+      </c>
+      <c r="K12" s="27">
+        <v>-1.6132880761686019</v>
+      </c>
+      <c r="L12" s="27">
+        <v>-1.8791636507218989</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13">
+        <v>1993459.613516357</v>
+      </c>
+      <c r="C13" s="13">
+        <v>1991142.716078849</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1989601.208189657</v>
+      </c>
+      <c r="E13" s="13">
+        <v>1988837.9122553931</v>
+      </c>
+      <c r="F13" s="13">
+        <v>1987894.658411968</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="27">
+        <v>-0.1162249499211508</v>
+      </c>
+      <c r="J13" s="27">
+        <v>-0.1935532227760586</v>
+      </c>
+      <c r="K13" s="27">
+        <v>-0.23184323522921629</v>
+      </c>
+      <c r="L13" s="27">
+        <v>-0.27916066453800431</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="13">
+        <v>1209532.48903948</v>
+      </c>
+      <c r="C14" s="13">
+        <v>1199795.645888966</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1194876.7203289799</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1190960.3980956699</v>
+      </c>
+      <c r="F14" s="13">
+        <v>1187636.052603103</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="27">
+        <v>-0.80500881445908479</v>
+      </c>
+      <c r="J14" s="27">
+        <v>-1.211688718021857</v>
+      </c>
+      <c r="K14" s="27">
+        <v>-1.535476815389939</v>
+      </c>
+      <c r="L14" s="27">
+        <v>-1.810322305088782</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="13">
+        <v>848111.70255372697</v>
+      </c>
+      <c r="C15" s="13">
+        <v>837187.76180597779</v>
+      </c>
+      <c r="D15" s="13">
+        <v>830311.32811358734</v>
+      </c>
+      <c r="E15" s="13">
+        <v>825489.36248479248</v>
+      </c>
+      <c r="F15" s="13">
+        <v>821592.0268113811</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="27">
+        <v>-1.2880308943805849</v>
+      </c>
+      <c r="J15" s="27">
+        <v>-2.0988242924300402</v>
+      </c>
+      <c r="K15" s="27">
+        <v>-2.6673774221976831</v>
+      </c>
+      <c r="L15" s="27">
+        <v>-3.1269083615393072</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="13">
+        <v>450023.70084612112</v>
+      </c>
+      <c r="C16" s="13">
+        <v>445919.93565351359</v>
+      </c>
+      <c r="D16" s="13">
+        <v>443710.5555951579</v>
+      </c>
+      <c r="E16" s="13">
+        <v>442004.56013159722</v>
+      </c>
+      <c r="F16" s="13">
+        <v>440612.6737071859</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="27">
+        <v>-0.91189979214244876</v>
+      </c>
+      <c r="J16" s="27">
+        <v>-1.4028472809528549</v>
+      </c>
+      <c r="K16" s="27">
+        <v>-1.781937417839673</v>
+      </c>
+      <c r="L16" s="27">
+        <v>-2.0912292222033848</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="14">
+        <v>545780.89723545057</v>
+      </c>
+      <c r="C17" s="14">
+        <v>541529.11506716756</v>
+      </c>
+      <c r="D17" s="14">
+        <v>540641.74227424012</v>
+      </c>
+      <c r="E17" s="14">
+        <v>539281.02177879063</v>
+      </c>
+      <c r="F17" s="14">
+        <v>538165.00742780615</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="28">
+        <v>-0.77902729645167235</v>
+      </c>
+      <c r="J17" s="28">
+        <v>-0.94161503036142447</v>
+      </c>
+      <c r="K17" s="28">
+        <v>-1.190931285719933</v>
+      </c>
+      <c r="L17" s="28">
+        <v>-1.3954115738057631</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE9D1D0-DA06-4400-80F7-212E7ABF5402}">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:L17"/>
     </sheetView>
   </sheetViews>
@@ -8164,7 +8789,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>27</v>
@@ -8199,34 +8824,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="11">
-        <v>3414557.6450926722</v>
+        <v>1</v>
       </c>
       <c r="C2" s="11">
-        <v>3371922.167440231</v>
+        <v>1.006793512631031</v>
       </c>
       <c r="D2" s="11">
-        <v>3341541.9131478579</v>
+        <v>1.012917769932079</v>
       </c>
       <c r="E2" s="11">
-        <v>3321503.50550575</v>
+        <v>1.0166861217181911</v>
       </c>
       <c r="F2" s="11">
-        <v>3305970.940609239</v>
-      </c>
-      <c r="H2" s="27" t="s">
+        <v>1.0195515499697201</v>
+      </c>
+      <c r="H2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="24">
-        <v>-1.2486383913803889</v>
-      </c>
-      <c r="J2" s="24">
-        <v>-2.1383657719104829</v>
-      </c>
-      <c r="K2" s="24">
-        <v>-2.7252180006583622</v>
-      </c>
-      <c r="L2" s="24">
-        <v>-3.1801104497237471</v>
+      <c r="I2" s="26">
+        <v>0.67935126310307847</v>
+      </c>
+      <c r="J2" s="26">
+        <v>1.2917769932079051</v>
+      </c>
+      <c r="K2" s="26">
+        <v>1.668612171819106</v>
+      </c>
+      <c r="L2" s="26">
+        <v>1.9551549969719859</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -8234,34 +8859,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="13">
-        <v>236483.0463515812</v>
+        <v>1</v>
       </c>
       <c r="C3" s="13">
-        <v>226665.5223881923</v>
+        <v>1.0053148965906611</v>
       </c>
       <c r="D3" s="13">
-        <v>227221.33319504379</v>
+        <v>1.003798874193214</v>
       </c>
       <c r="E3" s="13">
-        <v>224487.88262577329</v>
+        <v>1.00503360265802</v>
       </c>
       <c r="F3" s="13">
-        <v>222151.59597603261</v>
-      </c>
-      <c r="H3" s="27" t="s">
+        <v>1.0061509444978629</v>
+      </c>
+      <c r="H3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="25">
-        <v>-4.1514705239347727</v>
-      </c>
-      <c r="J3" s="25">
-        <v>-3.91643853520387</v>
-      </c>
-      <c r="K3" s="25">
-        <v>-5.0723144474274706</v>
-      </c>
-      <c r="L3" s="25">
-        <v>-6.0602443163058473</v>
+      <c r="I3" s="27">
+        <v>0.5314896590661311</v>
+      </c>
+      <c r="J3" s="27">
+        <v>0.37988741932137859</v>
+      </c>
+      <c r="K3" s="27">
+        <v>0.50336026580204418</v>
+      </c>
+      <c r="L3" s="27">
+        <v>0.61509444978633532</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -8269,34 +8894,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="13">
-        <v>10693184.370907759</v>
+        <v>1</v>
       </c>
       <c r="C4" s="13">
-        <v>10582916.886244269</v>
+        <v>1.0006148314528269</v>
       </c>
       <c r="D4" s="13">
-        <v>10509452.422878619</v>
+        <v>1.001162373313975</v>
       </c>
       <c r="E4" s="13">
-        <v>10459697.821077229</v>
+        <v>1.0014870634100901</v>
       </c>
       <c r="F4" s="13">
-        <v>10420343.124573519</v>
-      </c>
-      <c r="H4" s="27" t="s">
+        <v>1.001743645504285</v>
+      </c>
+      <c r="H4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="25">
-        <v>-1.0311940843691769</v>
-      </c>
-      <c r="J4" s="25">
-        <v>-1.7182154693695459</v>
-      </c>
-      <c r="K4" s="25">
-        <v>-2.183508127529918</v>
-      </c>
-      <c r="L4" s="25">
-        <v>-2.5515434586215591</v>
+      <c r="I4" s="27">
+        <v>6.1483145282670293E-2</v>
+      </c>
+      <c r="J4" s="27">
+        <v>0.1162373313974507</v>
+      </c>
+      <c r="K4" s="27">
+        <v>0.1487063410090084</v>
+      </c>
+      <c r="L4" s="27">
+        <v>0.17436455042851851</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -8304,34 +8929,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="13">
-        <v>859555.56858298206</v>
+        <v>1</v>
       </c>
       <c r="C5" s="13">
-        <v>850694.24528555304</v>
+        <v>1.0048862261331</v>
       </c>
       <c r="D5" s="13">
-        <v>845128.35955597402</v>
+        <v>1.008459584605764</v>
       </c>
       <c r="E5" s="13">
-        <v>841300.77145803953</v>
+        <v>1.010567877235488</v>
       </c>
       <c r="F5" s="13">
-        <v>838157.32115848304</v>
-      </c>
-      <c r="H5" s="27" t="s">
+        <v>1.0126732860578029</v>
+      </c>
+      <c r="H5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="25">
-        <v>-1.030919189091791</v>
-      </c>
-      <c r="J5" s="25">
-        <v>-1.678449835511155</v>
-      </c>
-      <c r="K5" s="25">
-        <v>-2.123748340672893</v>
-      </c>
-      <c r="L5" s="25">
-        <v>-2.489454807415771</v>
+      <c r="I5" s="27">
+        <v>0.48862261331004131</v>
+      </c>
+      <c r="J5" s="27">
+        <v>0.84595846057635704</v>
+      </c>
+      <c r="K5" s="27">
+        <v>1.0567877235487579</v>
+      </c>
+      <c r="L5" s="27">
+        <v>1.2673286057802711</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -8339,34 +8964,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="13">
-        <v>2955558.9711368098</v>
+        <v>1</v>
       </c>
       <c r="C6" s="13">
-        <v>2929607.8739666371</v>
+        <v>1.0044124889013271</v>
       </c>
       <c r="D6" s="13">
-        <v>2911148.510167181</v>
+        <v>1.0081943577466219</v>
       </c>
       <c r="E6" s="13">
-        <v>2899175.4909311002</v>
+        <v>1.0104476900192421</v>
       </c>
       <c r="F6" s="13">
-        <v>2888980.153776777</v>
-      </c>
-      <c r="H6" s="27" t="s">
+        <v>1.012511883395971</v>
+      </c>
+      <c r="H6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="25">
-        <v>-0.87804362638689082</v>
-      </c>
-      <c r="J6" s="25">
-        <v>-1.502607845193729</v>
-      </c>
-      <c r="K6" s="25">
-        <v>-1.907709531643097</v>
-      </c>
-      <c r="L6" s="25">
-        <v>-2.252664149496697</v>
+      <c r="I6" s="27">
+        <v>0.44124889013272828</v>
+      </c>
+      <c r="J6" s="27">
+        <v>0.81943577466219164</v>
+      </c>
+      <c r="K6" s="27">
+        <v>1.044769001924206</v>
+      </c>
+      <c r="L6" s="27">
+        <v>1.251188339597076</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -8374,34 +8999,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="13">
-        <v>4193101.5613005492</v>
+        <v>1</v>
       </c>
       <c r="C7" s="13">
-        <v>4154337.916997124</v>
+        <v>1.000908368828781</v>
       </c>
       <c r="D7" s="13">
-        <v>4129223.5030272719</v>
+        <v>1.0016865944369291</v>
       </c>
       <c r="E7" s="13">
-        <v>4112278.113780838</v>
+        <v>1.0020525062501811</v>
       </c>
       <c r="F7" s="13">
-        <v>4099208.7994941161</v>
-      </c>
-      <c r="H7" s="27" t="s">
+        <v>1.0022260059102099</v>
+      </c>
+      <c r="H7" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="25">
-        <v>-0.92446232786697857</v>
-      </c>
-      <c r="J7" s="25">
-        <v>-1.5234083253033479</v>
-      </c>
-      <c r="K7" s="25">
-        <v>-1.92753374413003</v>
-      </c>
-      <c r="L7" s="25">
-        <v>-2.2392198336667861</v>
+      <c r="I7" s="27">
+        <v>9.0836882878120306E-2</v>
+      </c>
+      <c r="J7" s="27">
+        <v>0.16865944369286459</v>
+      </c>
+      <c r="K7" s="27">
+        <v>0.2052506250181052</v>
+      </c>
+      <c r="L7" s="27">
+        <v>0.22260059102101601</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -8409,34 +9034,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="13">
-        <v>1706212.1311634949</v>
+        <v>1</v>
       </c>
       <c r="C8" s="13">
-        <v>1685403.804716252</v>
+        <v>1.0023475505750179</v>
       </c>
       <c r="D8" s="13">
-        <v>1676461.958796306</v>
+        <v>1.00249362696532</v>
       </c>
       <c r="E8" s="13">
-        <v>1668390.1823580919</v>
+        <v>1.003201308149122</v>
       </c>
       <c r="F8" s="13">
-        <v>1661980.2115839471</v>
-      </c>
-      <c r="H8" s="27" t="s">
+        <v>1.003783197101296</v>
+      </c>
+      <c r="H8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="25">
-        <v>-1.2195626831614159</v>
-      </c>
-      <c r="J8" s="25">
-        <v>-1.7436385443409941</v>
-      </c>
-      <c r="K8" s="25">
-        <v>-2.2167201905669121</v>
-      </c>
-      <c r="L8" s="25">
-        <v>-2.5924044713821921</v>
+      <c r="I8" s="27">
+        <v>0.234755057501812</v>
+      </c>
+      <c r="J8" s="27">
+        <v>0.2493626965320184</v>
+      </c>
+      <c r="K8" s="27">
+        <v>0.32013081491217837</v>
+      </c>
+      <c r="L8" s="27">
+        <v>0.37831971012955989</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -8444,34 +9069,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="13">
-        <v>1023361.531720356</v>
+        <v>1</v>
       </c>
       <c r="C9" s="13">
-        <v>1012958.540185417</v>
+        <v>1.0004503224587791</v>
       </c>
       <c r="D9" s="13">
-        <v>1001988.3664715179</v>
+        <v>1.001636849992205</v>
       </c>
       <c r="E9" s="13">
-        <v>996378.48776528169</v>
+        <v>1.002059458994091</v>
       </c>
       <c r="F9" s="13">
-        <v>992376.37968712253</v>
-      </c>
-      <c r="H9" s="27" t="s">
+        <v>1.002317138439438</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="25">
-        <v>-1.016550965859581</v>
-      </c>
-      <c r="J9" s="25">
-        <v>-2.0885253731306759</v>
-      </c>
-      <c r="K9" s="25">
-        <v>-2.6367068839995902</v>
-      </c>
-      <c r="L9" s="25">
-        <v>-3.0277815877195242</v>
+      <c r="I9" s="27">
+        <v>4.5032245877929533E-2</v>
+      </c>
+      <c r="J9" s="27">
+        <v>0.16368499922048141</v>
+      </c>
+      <c r="K9" s="27">
+        <v>0.20594589940907679</v>
+      </c>
+      <c r="L9" s="27">
+        <v>0.23171384394375941</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -8479,34 +9104,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="13">
-        <v>1008230.237982081</v>
+        <v>1</v>
       </c>
       <c r="C10" s="13">
-        <v>999576.21799253311</v>
+        <v>1.0002883997378571</v>
       </c>
       <c r="D10" s="13">
-        <v>993776.97677164082</v>
+        <v>1.0008872351841169</v>
       </c>
       <c r="E10" s="13">
-        <v>989860.45310062566</v>
+        <v>1.0011499607302461</v>
       </c>
       <c r="F10" s="13">
-        <v>986770.41759965976</v>
-      </c>
-      <c r="H10" s="27" t="s">
+        <v>1.001348230429324</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="25">
-        <v>-0.85833767561548846</v>
-      </c>
-      <c r="J10" s="25">
-        <v>-1.4335278457198051</v>
-      </c>
-      <c r="K10" s="25">
-        <v>-1.821983133358656</v>
-      </c>
-      <c r="L10" s="25">
-        <v>-2.1284642707574348</v>
+      <c r="I10" s="27">
+        <v>2.8839973785710349E-2</v>
+      </c>
+      <c r="J10" s="27">
+        <v>8.8723518411693014E-2</v>
+      </c>
+      <c r="K10" s="27">
+        <v>0.11499607302458691</v>
+      </c>
+      <c r="L10" s="27">
+        <v>0.13482304293244149</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -8514,34 +9139,34 @@
         <v>10</v>
       </c>
       <c r="B11" s="13">
-        <v>2590209.541191509</v>
+        <v>1</v>
       </c>
       <c r="C11" s="13">
-        <v>2570935.8422241178</v>
+        <v>0.99876982636797706</v>
       </c>
       <c r="D11" s="13">
-        <v>2560737.5522944559</v>
+        <v>0.99729562129493587</v>
       </c>
       <c r="E11" s="13">
-        <v>2552921.4062267612</v>
+        <v>0.99649538557265627</v>
       </c>
       <c r="F11" s="13">
-        <v>2546392.320697932</v>
-      </c>
-      <c r="H11" s="27" t="s">
+        <v>0.99602838625735035</v>
+      </c>
+      <c r="H11" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="25">
-        <v>-0.74409806082812757</v>
-      </c>
-      <c r="J11" s="25">
-        <v>-1.137822574906268</v>
-      </c>
-      <c r="K11" s="25">
-        <v>-1.4395798630096761</v>
-      </c>
-      <c r="L11" s="25">
-        <v>-1.6916477140849879</v>
+      <c r="I11" s="27">
+        <v>-0.12301736320229351</v>
+      </c>
+      <c r="J11" s="27">
+        <v>-0.27043787050641249</v>
+      </c>
+      <c r="K11" s="27">
+        <v>-0.3504614427343733</v>
+      </c>
+      <c r="L11" s="27">
+        <v>-0.39716137426496489</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -8549,34 +9174,34 @@
         <v>11</v>
       </c>
       <c r="B12" s="13">
-        <v>1427752.6162607169</v>
+        <v>1</v>
       </c>
       <c r="C12" s="13">
-        <v>1416760.3461790089</v>
+        <v>0.99948953640426397</v>
       </c>
       <c r="D12" s="13">
-        <v>1409554.0075849199</v>
+        <v>0.9999122537008962</v>
       </c>
       <c r="E12" s="13">
-        <v>1404718.853545398</v>
+        <v>0.99984109256913878</v>
       </c>
       <c r="F12" s="13">
-        <v>1400922.8080737151</v>
-      </c>
-      <c r="H12" s="27" t="s">
+        <v>0.99974891627420936</v>
+      </c>
+      <c r="H12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="25">
-        <v>-0.76990018834614049</v>
-      </c>
-      <c r="J12" s="25">
-        <v>-1.2746331870474441</v>
-      </c>
-      <c r="K12" s="25">
-        <v>-1.6132880761686019</v>
-      </c>
-      <c r="L12" s="25">
-        <v>-1.8791636507218989</v>
+      <c r="I12" s="27">
+        <v>-5.1046359573603262E-2</v>
+      </c>
+      <c r="J12" s="27">
+        <v>-8.7746299103796943E-3</v>
+      </c>
+      <c r="K12" s="27">
+        <v>-1.589074308612215E-2</v>
+      </c>
+      <c r="L12" s="27">
+        <v>-2.5108372579063509E-2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -8584,34 +9209,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="13">
-        <v>1993459.613516357</v>
+        <v>1</v>
       </c>
       <c r="C13" s="13">
-        <v>1991142.716078849</v>
+        <v>0.99501288039461622</v>
       </c>
       <c r="D13" s="13">
-        <v>1989601.208189657</v>
+        <v>0.99212034660887516</v>
       </c>
       <c r="E13" s="13">
-        <v>1988837.9122553931</v>
+        <v>0.98992436344360857</v>
       </c>
       <c r="F13" s="13">
-        <v>1987894.658411968</v>
-      </c>
-      <c r="H13" s="27" t="s">
+        <v>0.98827503641633296</v>
+      </c>
+      <c r="H13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="25">
-        <v>-0.1162249499211508</v>
-      </c>
-      <c r="J13" s="25">
-        <v>-0.1935532227760586</v>
-      </c>
-      <c r="K13" s="25">
-        <v>-0.23184323522921629</v>
-      </c>
-      <c r="L13" s="25">
-        <v>-0.27916066453800431</v>
+      <c r="I13" s="27">
+        <v>-0.4987119605383783</v>
+      </c>
+      <c r="J13" s="27">
+        <v>-0.78796533911248412</v>
+      </c>
+      <c r="K13" s="27">
+        <v>-1.007563655639143</v>
+      </c>
+      <c r="L13" s="27">
+        <v>-1.1724963583667041</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -8619,34 +9244,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="13">
-        <v>1209532.48903948</v>
+        <v>1</v>
       </c>
       <c r="C14" s="13">
-        <v>1199795.645888966</v>
+        <v>1.0001441228562129</v>
       </c>
       <c r="D14" s="13">
-        <v>1194876.7203289799</v>
+        <v>0.99958063770216132</v>
       </c>
       <c r="E14" s="13">
-        <v>1190960.3980956699</v>
+        <v>0.99943587891029384</v>
       </c>
       <c r="F14" s="13">
-        <v>1187636.052603103</v>
-      </c>
-      <c r="H14" s="27" t="s">
+        <v>0.99951767325548246</v>
+      </c>
+      <c r="H14" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="25">
-        <v>-0.80500881445908479</v>
-      </c>
-      <c r="J14" s="25">
-        <v>-1.211688718021857</v>
-      </c>
-      <c r="K14" s="25">
-        <v>-1.535476815389939</v>
-      </c>
-      <c r="L14" s="25">
-        <v>-1.810322305088782</v>
+      <c r="I14" s="27">
+        <v>1.441228562129027E-2</v>
+      </c>
+      <c r="J14" s="27">
+        <v>-4.1936229783867678E-2</v>
+      </c>
+      <c r="K14" s="27">
+        <v>-5.6412108970615993E-2</v>
+      </c>
+      <c r="L14" s="27">
+        <v>-4.823267445175361E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -8654,34 +9279,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="13">
-        <v>848111.70255372697</v>
+        <v>1</v>
       </c>
       <c r="C15" s="13">
-        <v>837187.76180597779</v>
+        <v>1.0052137580091449</v>
       </c>
       <c r="D15" s="13">
-        <v>830311.32811358734</v>
+        <v>1.008953129550731</v>
       </c>
       <c r="E15" s="13">
-        <v>825489.36248479248</v>
+        <v>1.0114747019397261</v>
       </c>
       <c r="F15" s="13">
-        <v>821592.0268113811</v>
-      </c>
-      <c r="H15" s="27" t="s">
+        <v>1.013604556016358</v>
+      </c>
+      <c r="H15" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="25">
-        <v>-1.2880308943805849</v>
-      </c>
-      <c r="J15" s="25">
-        <v>-2.0988242924300402</v>
-      </c>
-      <c r="K15" s="25">
-        <v>-2.6673774221976831</v>
-      </c>
-      <c r="L15" s="25">
-        <v>-3.1269083615393072</v>
+      <c r="I15" s="27">
+        <v>0.52137580091453639</v>
+      </c>
+      <c r="J15" s="27">
+        <v>0.89531295507314645</v>
+      </c>
+      <c r="K15" s="27">
+        <v>1.1474701939726111</v>
+      </c>
+      <c r="L15" s="27">
+        <v>1.3604556016357789</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -8689,34 +9314,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="13">
-        <v>450023.70084612112</v>
+        <v>1</v>
       </c>
       <c r="C16" s="13">
-        <v>445919.93565351359</v>
+        <v>1.0013206648456929</v>
       </c>
       <c r="D16" s="13">
-        <v>443710.5555951579</v>
+        <v>1.001668892972801</v>
       </c>
       <c r="E16" s="13">
-        <v>442004.56013159722</v>
+        <v>1.0021373425458939</v>
       </c>
       <c r="F16" s="13">
-        <v>440612.6737071859</v>
-      </c>
-      <c r="H16" s="27" t="s">
+        <v>1.0026263687291741</v>
+      </c>
+      <c r="H16" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="25">
-        <v>-0.91189979214244876</v>
-      </c>
-      <c r="J16" s="25">
-        <v>-1.4028472809528549</v>
-      </c>
-      <c r="K16" s="25">
-        <v>-1.781937417839673</v>
-      </c>
-      <c r="L16" s="25">
-        <v>-2.0912292222033848</v>
+      <c r="I16" s="27">
+        <v>0.13206648456931541</v>
+      </c>
+      <c r="J16" s="27">
+        <v>0.1668892972801039</v>
+      </c>
+      <c r="K16" s="27">
+        <v>0.21373425458937059</v>
+      </c>
+      <c r="L16" s="27">
+        <v>0.2626368729173878</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -8724,628 +9349,6 @@
         <v>16</v>
       </c>
       <c r="B17" s="14">
-        <v>545780.89723545057</v>
-      </c>
-      <c r="C17" s="14">
-        <v>541529.11506716756</v>
-      </c>
-      <c r="D17" s="14">
-        <v>540641.74227424012</v>
-      </c>
-      <c r="E17" s="14">
-        <v>539281.02177879063</v>
-      </c>
-      <c r="F17" s="14">
-        <v>538165.00742780615</v>
-      </c>
-      <c r="H17" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="26">
-        <v>-0.77902729645167235</v>
-      </c>
-      <c r="J17" s="26">
-        <v>-0.94161503036142447</v>
-      </c>
-      <c r="K17" s="26">
-        <v>-1.190931285719933</v>
-      </c>
-      <c r="L17" s="26">
-        <v>-1.3954115738057631</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE9D1D0-DA06-4400-80F7-212E7ABF5402}">
-  <dimension ref="A1:L17"/>
-  <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11">
-        <v>1.006793512631031</v>
-      </c>
-      <c r="D2" s="11">
-        <v>1.012917769932079</v>
-      </c>
-      <c r="E2" s="11">
-        <v>1.0166861217181911</v>
-      </c>
-      <c r="F2" s="11">
-        <v>1.0195515499697201</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="24">
-        <v>0.67935126310307847</v>
-      </c>
-      <c r="J2" s="24">
-        <v>1.2917769932079051</v>
-      </c>
-      <c r="K2" s="24">
-        <v>1.668612171819106</v>
-      </c>
-      <c r="L2" s="24">
-        <v>1.9551549969719859</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="13">
-        <v>1</v>
-      </c>
-      <c r="C3" s="13">
-        <v>1.0053148965906611</v>
-      </c>
-      <c r="D3" s="13">
-        <v>1.003798874193214</v>
-      </c>
-      <c r="E3" s="13">
-        <v>1.00503360265802</v>
-      </c>
-      <c r="F3" s="13">
-        <v>1.0061509444978629</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="25">
-        <v>0.5314896590661311</v>
-      </c>
-      <c r="J3" s="25">
-        <v>0.37988741932137859</v>
-      </c>
-      <c r="K3" s="25">
-        <v>0.50336026580204418</v>
-      </c>
-      <c r="L3" s="25">
-        <v>0.61509444978633532</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="13">
-        <v>1</v>
-      </c>
-      <c r="C4" s="13">
-        <v>1.0006148314528269</v>
-      </c>
-      <c r="D4" s="13">
-        <v>1.001162373313975</v>
-      </c>
-      <c r="E4" s="13">
-        <v>1.0014870634100901</v>
-      </c>
-      <c r="F4" s="13">
-        <v>1.001743645504285</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="25">
-        <v>6.1483145282670293E-2</v>
-      </c>
-      <c r="J4" s="25">
-        <v>0.1162373313974507</v>
-      </c>
-      <c r="K4" s="25">
-        <v>0.1487063410090084</v>
-      </c>
-      <c r="L4" s="25">
-        <v>0.17436455042851851</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13">
-        <v>1</v>
-      </c>
-      <c r="C5" s="13">
-        <v>1.0048862261331</v>
-      </c>
-      <c r="D5" s="13">
-        <v>1.008459584605764</v>
-      </c>
-      <c r="E5" s="13">
-        <v>1.010567877235488</v>
-      </c>
-      <c r="F5" s="13">
-        <v>1.0126732860578029</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="25">
-        <v>0.48862261331004131</v>
-      </c>
-      <c r="J5" s="25">
-        <v>0.84595846057635704</v>
-      </c>
-      <c r="K5" s="25">
-        <v>1.0567877235487579</v>
-      </c>
-      <c r="L5" s="25">
-        <v>1.2673286057802711</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="13">
-        <v>1</v>
-      </c>
-      <c r="C6" s="13">
-        <v>1.0044124889013271</v>
-      </c>
-      <c r="D6" s="13">
-        <v>1.0081943577466219</v>
-      </c>
-      <c r="E6" s="13">
-        <v>1.0104476900192421</v>
-      </c>
-      <c r="F6" s="13">
-        <v>1.012511883395971</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="25">
-        <v>0.44124889013272828</v>
-      </c>
-      <c r="J6" s="25">
-        <v>0.81943577466219164</v>
-      </c>
-      <c r="K6" s="25">
-        <v>1.044769001924206</v>
-      </c>
-      <c r="L6" s="25">
-        <v>1.251188339597076</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13">
-        <v>1</v>
-      </c>
-      <c r="C7" s="13">
-        <v>1.000908368828781</v>
-      </c>
-      <c r="D7" s="13">
-        <v>1.0016865944369291</v>
-      </c>
-      <c r="E7" s="13">
-        <v>1.0020525062501811</v>
-      </c>
-      <c r="F7" s="13">
-        <v>1.0022260059102099</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="25">
-        <v>9.0836882878120306E-2</v>
-      </c>
-      <c r="J7" s="25">
-        <v>0.16865944369286459</v>
-      </c>
-      <c r="K7" s="25">
-        <v>0.2052506250181052</v>
-      </c>
-      <c r="L7" s="25">
-        <v>0.22260059102101601</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="13">
-        <v>1</v>
-      </c>
-      <c r="C8" s="13">
-        <v>1.0023475505750179</v>
-      </c>
-      <c r="D8" s="13">
-        <v>1.00249362696532</v>
-      </c>
-      <c r="E8" s="13">
-        <v>1.003201308149122</v>
-      </c>
-      <c r="F8" s="13">
-        <v>1.003783197101296</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="25">
-        <v>0.234755057501812</v>
-      </c>
-      <c r="J8" s="25">
-        <v>0.2493626965320184</v>
-      </c>
-      <c r="K8" s="25">
-        <v>0.32013081491217837</v>
-      </c>
-      <c r="L8" s="25">
-        <v>0.37831971012955989</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="13">
-        <v>1</v>
-      </c>
-      <c r="C9" s="13">
-        <v>1.0004503224587791</v>
-      </c>
-      <c r="D9" s="13">
-        <v>1.001636849992205</v>
-      </c>
-      <c r="E9" s="13">
-        <v>1.002059458994091</v>
-      </c>
-      <c r="F9" s="13">
-        <v>1.002317138439438</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="25">
-        <v>4.5032245877929533E-2</v>
-      </c>
-      <c r="J9" s="25">
-        <v>0.16368499922048141</v>
-      </c>
-      <c r="K9" s="25">
-        <v>0.20594589940907679</v>
-      </c>
-      <c r="L9" s="25">
-        <v>0.23171384394375941</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="13">
-        <v>1</v>
-      </c>
-      <c r="C10" s="13">
-        <v>1.0002883997378571</v>
-      </c>
-      <c r="D10" s="13">
-        <v>1.0008872351841169</v>
-      </c>
-      <c r="E10" s="13">
-        <v>1.0011499607302461</v>
-      </c>
-      <c r="F10" s="13">
-        <v>1.001348230429324</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="25">
-        <v>2.8839973785710349E-2</v>
-      </c>
-      <c r="J10" s="25">
-        <v>8.8723518411693014E-2</v>
-      </c>
-      <c r="K10" s="25">
-        <v>0.11499607302458691</v>
-      </c>
-      <c r="L10" s="25">
-        <v>0.13482304293244149</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="13">
-        <v>1</v>
-      </c>
-      <c r="C11" s="13">
-        <v>0.99876982636797706</v>
-      </c>
-      <c r="D11" s="13">
-        <v>0.99729562129493587</v>
-      </c>
-      <c r="E11" s="13">
-        <v>0.99649538557265627</v>
-      </c>
-      <c r="F11" s="13">
-        <v>0.99602838625735035</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="25">
-        <v>-0.12301736320229351</v>
-      </c>
-      <c r="J11" s="25">
-        <v>-0.27043787050641249</v>
-      </c>
-      <c r="K11" s="25">
-        <v>-0.3504614427343733</v>
-      </c>
-      <c r="L11" s="25">
-        <v>-0.39716137426496489</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="13">
-        <v>1</v>
-      </c>
-      <c r="C12" s="13">
-        <v>0.99948953640426397</v>
-      </c>
-      <c r="D12" s="13">
-        <v>0.9999122537008962</v>
-      </c>
-      <c r="E12" s="13">
-        <v>0.99984109256913878</v>
-      </c>
-      <c r="F12" s="13">
-        <v>0.99974891627420936</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="25">
-        <v>-5.1046359573603262E-2</v>
-      </c>
-      <c r="J12" s="25">
-        <v>-8.7746299103796943E-3</v>
-      </c>
-      <c r="K12" s="25">
-        <v>-1.589074308612215E-2</v>
-      </c>
-      <c r="L12" s="25">
-        <v>-2.5108372579063509E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="13">
-        <v>0.99501288039461622</v>
-      </c>
-      <c r="D13" s="13">
-        <v>0.99212034660887516</v>
-      </c>
-      <c r="E13" s="13">
-        <v>0.98992436344360857</v>
-      </c>
-      <c r="F13" s="13">
-        <v>0.98827503641633296</v>
-      </c>
-      <c r="H13" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" s="25">
-        <v>-0.4987119605383783</v>
-      </c>
-      <c r="J13" s="25">
-        <v>-0.78796533911248412</v>
-      </c>
-      <c r="K13" s="25">
-        <v>-1.007563655639143</v>
-      </c>
-      <c r="L13" s="25">
-        <v>-1.1724963583667041</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="13">
-        <v>1</v>
-      </c>
-      <c r="C14" s="13">
-        <v>1.0001441228562129</v>
-      </c>
-      <c r="D14" s="13">
-        <v>0.99958063770216132</v>
-      </c>
-      <c r="E14" s="13">
-        <v>0.99943587891029384</v>
-      </c>
-      <c r="F14" s="13">
-        <v>0.99951767325548246</v>
-      </c>
-      <c r="H14" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="25">
-        <v>1.441228562129027E-2</v>
-      </c>
-      <c r="J14" s="25">
-        <v>-4.1936229783867678E-2</v>
-      </c>
-      <c r="K14" s="25">
-        <v>-5.6412108970615993E-2</v>
-      </c>
-      <c r="L14" s="25">
-        <v>-4.823267445175361E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="13">
-        <v>1</v>
-      </c>
-      <c r="C15" s="13">
-        <v>1.0052137580091449</v>
-      </c>
-      <c r="D15" s="13">
-        <v>1.008953129550731</v>
-      </c>
-      <c r="E15" s="13">
-        <v>1.0114747019397261</v>
-      </c>
-      <c r="F15" s="13">
-        <v>1.013604556016358</v>
-      </c>
-      <c r="H15" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="25">
-        <v>0.52137580091453639</v>
-      </c>
-      <c r="J15" s="25">
-        <v>0.89531295507314645</v>
-      </c>
-      <c r="K15" s="25">
-        <v>1.1474701939726111</v>
-      </c>
-      <c r="L15" s="25">
-        <v>1.3604556016357789</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="13">
-        <v>1</v>
-      </c>
-      <c r="C16" s="13">
-        <v>1.0013206648456929</v>
-      </c>
-      <c r="D16" s="13">
-        <v>1.001668892972801</v>
-      </c>
-      <c r="E16" s="13">
-        <v>1.0021373425458939</v>
-      </c>
-      <c r="F16" s="13">
-        <v>1.0026263687291741</v>
-      </c>
-      <c r="H16" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="25">
-        <v>0.13206648456931541</v>
-      </c>
-      <c r="J16" s="25">
-        <v>0.1668892972801039</v>
-      </c>
-      <c r="K16" s="25">
-        <v>0.21373425458937059</v>
-      </c>
-      <c r="L16" s="25">
-        <v>0.2626368729173878</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="14">
         <v>1</v>
       </c>
       <c r="C17" s="14">
@@ -9360,20 +9363,26 @@
       <c r="F17" s="14">
         <v>0.99627262771394098</v>
       </c>
-      <c r="H17" s="28" t="s">
+      <c r="H17" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="26">
+      <c r="I17" s="28">
         <v>-1.2714799091040341E-3</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J17" s="28">
         <v>-0.25143976035069132</v>
       </c>
-      <c r="K17" s="26">
+      <c r="K17" s="28">
         <v>-0.32341944946795431</v>
       </c>
-      <c r="L17" s="26">
+      <c r="L17" s="28">
         <v>-0.37273722860590158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <f>1*0.68</f>
+        <v>0.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>